<commit_message>
A few tasks from lab_9
</commit_message>
<xml_diff>
--- a/Our_Labs/Lab_9/obliczenia_lab_9.xlsx
+++ b/Our_Labs/Lab_9/obliczenia_lab_9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\OneDrive\Pulpit\Szkoła\fizyka\moje_sprawka\repo\Fizyka\Our_Labs\Lab_9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryzen\Desktop\Git_repos\Fizyka\Our_Labs\Lab_9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80870E99-DA81-4AB1-BD2E-5E8D42FE4001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD31238A-7AED-4D6B-BC48-446735F4F9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -51,70 +51,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>, V</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>, V</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>f</t>
     </r>
     <r>
@@ -146,6 +82,56 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>, V</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -823,7 +809,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1702763871"/>
@@ -885,7 +871,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1709057647"/>
@@ -933,7 +919,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1448,7 +1434,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1702765855"/>
@@ -1510,7 +1496,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1709055247"/>
@@ -1558,7 +1544,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2073,7 +2059,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1651850863"/>
@@ -2136,7 +2122,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1697051663"/>
@@ -2184,7 +2170,1448 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11433554597381318"/>
+          <c:y val="2.2105579584198287E-2"/>
+          <c:w val="0.86208415849082942"/>
+          <c:h val="0.80843738748149696"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$C$5:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$D$5:$D$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>2.86E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.62E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.4199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.20699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.27979999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.59599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.66800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.70599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.74399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.78600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.82799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.872</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.91600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0820000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1459999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.198</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.1459999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.92600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.872</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.82199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.77800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.73599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.69799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.66400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.63200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.60399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.57799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.55400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.51200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.47599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.44400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.41799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.39400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.33700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.246</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.20799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.158</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0E6A-4008-8DBE-7DEE1F827F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$C$5:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$E$5:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.21</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.47</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0E6A-4008-8DBE-7DEE1F827F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$C$5:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$F$5:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0E6A-4008-8DBE-7DEE1F827F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1709057647"/>
+        <c:axId val="1702763871"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1709057647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1702763871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1702763871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1709057647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2316,6 +3743,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3349,6 +4816,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3969,6 +5952,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>80110</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>438698</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180071</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB1FC426-1DDB-4502-B138-EA943EC6EF9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4405,10 +6426,266 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.91392</cdr:x>
+      <cdr:y>0.93172</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.98647</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C68DF09-C545-2CD0-EDBD-CACAE30EE132}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5550776" y="3353649"/>
+          <a:ext cx="522812" cy="197069"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>f,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> kHz</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.00462</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.07355</cdr:x>
+      <cdr:y>0.13054</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="pole tekstowe 7">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F9CE7AA-B1A8-B56E-4CBC-FDC3DBE28DFC}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="16613"/>
+          <a:ext cx="446690" cy="453259"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.0119</cdr:x>
+      <cdr:y>0.03747</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.04867</cdr:x>
+      <cdr:y>0.09222</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="pole tekstowe 8">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07654D6A-0360-2AD9-44DB-B607B7F9FF12}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="72259" y="134854"/>
+          <a:ext cx="223344" cy="197069"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00216</cdr:x>
+      <cdr:y>0.00097</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.09953</cdr:x>
+      <cdr:y>0.18421</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="pole tekstowe 9">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF2E869-A61B-D37D-0874-CB94AB60E65D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="13137" y="3475"/>
+          <a:ext cx="591362" cy="659565"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>U</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>L</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>, V</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>U</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>, V</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>I, mA</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4446,7 +6723,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4552,7 +6829,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4694,7 +6971,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4704,13 +6981,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S52" sqref="S52"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X40" sqref="X40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4718,16 +6995,16 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" s="1">
         <v>144</v>
       </c>
@@ -4744,10 +7021,10 @@
         <v>1.85</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
@@ -4755,13 +7032,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>0.1</v>
       </c>
@@ -4775,7 +7052,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>0.2</v>
       </c>
@@ -4789,7 +7066,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>0.3</v>
       </c>
@@ -4803,7 +7080,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>0.4</v>
       </c>
@@ -4817,7 +7094,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>0.5</v>
       </c>
@@ -4831,7 +7108,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <v>0.6</v>
       </c>
@@ -4845,7 +7122,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>0.7</v>
       </c>
@@ -4859,7 +7136,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>0.8</v>
       </c>
@@ -4873,7 +7150,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>0.9</v>
       </c>
@@ -4887,7 +7164,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>1</v>
       </c>
@@ -4901,7 +7178,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -4915,7 +7192,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>1.2</v>
       </c>
@@ -4929,7 +7206,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>1.3</v>
       </c>
@@ -4943,7 +7220,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>1.4</v>
       </c>
@@ -4957,7 +7234,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>1.5</v>
       </c>
@@ -4971,7 +7248,7 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>1.6</v>
       </c>
@@ -4985,7 +7262,7 @@
         <v>2.09</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>1.65</v>
       </c>
@@ -4999,7 +7276,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>1.7</v>
       </c>
@@ -5013,7 +7290,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>1.75</v>
       </c>
@@ -5027,7 +7304,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>1.8</v>
       </c>
@@ -5041,7 +7318,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>1.85</v>
       </c>
@@ -5055,7 +7332,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>1.9</v>
       </c>
@@ -5069,7 +7346,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>1.95</v>
       </c>
@@ -5083,7 +7360,7 @@
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>2</v>
       </c>
@@ -5097,7 +7374,7 @@
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>2.0499999999999998</v>
       </c>
@@ -5111,7 +7388,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>2.1</v>
       </c>
@@ -5125,7 +7402,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -5139,7 +7416,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>2.2999999999999998</v>
       </c>
@@ -5153,7 +7430,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>2.4</v>
       </c>
@@ -5167,7 +7444,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>2.5</v>
       </c>
@@ -5181,7 +7458,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>2.6</v>
       </c>
@@ -5195,7 +7472,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>2.7</v>
       </c>
@@ -5209,7 +7486,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>2.8</v>
       </c>
@@ -5223,7 +7500,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>2.9</v>
       </c>
@@ -5237,7 +7514,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>3</v>
       </c>
@@ -5251,7 +7528,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>3.1</v>
       </c>
@@ -5265,7 +7542,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>3.2</v>
       </c>
@@ -5279,7 +7556,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>3.3</v>
       </c>
@@ -5293,7 +7570,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>3.4</v>
       </c>
@@ -5307,7 +7584,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>3.5</v>
       </c>
@@ -5321,7 +7598,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>3.6</v>
       </c>
@@ -5335,7 +7612,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>3.7</v>
       </c>
@@ -5349,7 +7626,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>3.8</v>
       </c>
@@ -5363,7 +7640,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>3.9</v>
       </c>
@@ -5377,7 +7654,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>4</v>
       </c>
@@ -5391,7 +7668,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>4.2</v>
       </c>
@@ -5405,7 +7682,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>4.4000000000000004</v>
       </c>
@@ -5419,7 +7696,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -5433,7 +7710,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>4.8</v>
       </c>
@@ -5447,7 +7724,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>5</v>
       </c>
@@ -5461,7 +7738,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>5.5</v>
       </c>
@@ -5475,7 +7752,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>6</v>
       </c>
@@ -5489,7 +7766,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>6.5</v>
       </c>
@@ -5503,7 +7780,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>7</v>
       </c>
@@ -5517,7 +7794,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>8</v>
       </c>
@@ -5531,7 +7808,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>9</v>
       </c>
@@ -5545,7 +7822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>10</v>
       </c>

</xml_diff>